<commit_message>
BUILD: updated didq sheet and readme
</commit_message>
<xml_diff>
--- a/Reports/didq_report.xlsx
+++ b/Reports/didq_report.xlsx
@@ -7,7 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="product_category_name_translati" sheetId="1" r:id="rId1"/>
+    <sheet name="closed_deals_data" sheetId="1" r:id="rId1"/>
+    <sheet name="customer_data" sheetId="2" r:id="rId2"/>
+    <sheet name="geolocation_data" sheetId="3" r:id="rId3"/>
+    <sheet name="marketing_leads_data" sheetId="4" r:id="rId4"/>
+    <sheet name="orders_data" sheetId="5" r:id="rId5"/>
+    <sheet name="orders_items_data" sheetId="6" r:id="rId6"/>
+    <sheet name="payments_data" sheetId="7" r:id="rId7"/>
+    <sheet name="reviews_data" sheetId="8" r:id="rId8"/>
+    <sheet name="products_data" sheetId="9" r:id="rId9"/>
+    <sheet name="sellers_data" sheetId="10" r:id="rId10"/>
+    <sheet name="products_names_data" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -891,6 +901,696 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>842</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>842</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>810</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>140</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>820</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5">
+        <v>133</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>824</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.001187648456057007</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>808</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>0.007125890736342043</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>833</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>332</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>177</v>
+      </c>
+      <c r="D9">
+        <v>0.2102137767220903</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>832</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>407</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>779</v>
+      </c>
+      <c r="D10">
+        <v>0.9251781472684085</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>839</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>58</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>778</v>
+      </c>
+      <c r="D11">
+        <v>0.9239904988123515</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>839</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>54</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>776</v>
+      </c>
+      <c r="D12">
+        <v>0.9216152019002375</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>835</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>0.01187648456057007</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>838</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13">
+        <v>587</v>
+      </c>
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>773</v>
+      </c>
+      <c r="D14">
+        <v>0.9180522565320665</v>
+      </c>
+      <c r="E14">
+        <v>33</v>
+      </c>
+      <c r="F14">
+        <v>808</v>
+      </c>
+      <c r="K14">
+        <v>233.0289855072464</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>2000</v>
+      </c>
+      <c r="N14">
+        <v>124172.0579710145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>815</v>
+      </c>
+      <c r="K15">
+        <v>73377.67933491686</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>50000000</v>
+      </c>
+      <c r="N15">
+        <v>3044324167681.025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3095</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2246</v>
+      </c>
+      <c r="F3">
+        <v>849</v>
+      </c>
+      <c r="K3">
+        <v>32291.05945072698</v>
+      </c>
+      <c r="L3">
+        <v>1001</v>
+      </c>
+      <c r="M3">
+        <v>99730</v>
+      </c>
+      <c r="N3">
+        <v>1070170061.455417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>611</v>
+      </c>
+      <c r="F4">
+        <v>2484</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4">
+        <v>694</v>
+      </c>
+      <c r="I4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>3072</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5">
+        <v>1849</v>
+      </c>
+      <c r="I5" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
@@ -952,25 +1652,134 @@
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3">
-        <v>32291.05945072698</v>
-      </c>
-      <c r="L3">
-        <v>1001</v>
-      </c>
-      <c r="M3">
-        <v>99730</v>
-      </c>
-      <c r="N3">
-        <v>1070170061.455417</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>99441</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>96096</v>
+      </c>
+      <c r="F3">
+        <v>3345</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -979,22 +1788,1721 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>611</v>
+        <v>14994</v>
       </c>
       <c r="F4">
-        <v>2484</v>
+        <v>84447</v>
+      </c>
+      <c r="K4">
+        <v>35137.47458291851</v>
+      </c>
+      <c r="L4">
+        <v>1003</v>
+      </c>
+      <c r="M4">
+        <v>99990</v>
+      </c>
+      <c r="N4">
+        <v>887917168.4216211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4119</v>
+      </c>
+      <c r="F5">
+        <v>95322</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5">
+        <v>15540</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>99414</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6">
+        <v>41746</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>19015</v>
+      </c>
+      <c r="F2">
+        <v>981148</v>
+      </c>
+      <c r="G2">
+        <v>36574.16646586607</v>
+      </c>
+      <c r="H2">
+        <v>1001</v>
+      </c>
+      <c r="I2">
+        <v>99990</v>
+      </c>
+      <c r="J2">
+        <v>933261912.3418242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>717360</v>
+      </c>
+      <c r="F3">
+        <v>282803</v>
+      </c>
+      <c r="G3">
+        <v>-21.17615291038396</v>
+      </c>
+      <c r="H3">
+        <v>-36.6053744107061</v>
+      </c>
+      <c r="I3">
+        <v>45.06593318269697</v>
+      </c>
+      <c r="J3">
+        <v>32.67112766033618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>717613</v>
+      </c>
+      <c r="F4">
+        <v>282550</v>
+      </c>
+      <c r="G4">
+        <v>-46.39054132093577</v>
+      </c>
+      <c r="H4">
+        <v>-101.4667664493148</v>
+      </c>
+      <c r="I4">
+        <v>121.1053938105776</v>
+      </c>
+      <c r="J4">
+        <v>18.23075060188097</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>8011</v>
+      </c>
+      <c r="F5">
+        <v>992152</v>
+      </c>
+      <c r="K5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5">
+        <v>135800</v>
+      </c>
+      <c r="M5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>1000136</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6">
+        <v>404268</v>
+      </c>
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6">
+        <v>646</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>8000</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>336</v>
+      </c>
+      <c r="F3">
+        <v>7664</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3">
+        <v>93</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>495</v>
+      </c>
+      <c r="F4">
+        <v>7505</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="H4">
-        <v>694</v>
+        <v>912</v>
       </c>
       <c r="I4" t="s">
-        <v>151</v>
+        <v>74</v>
       </c>
       <c r="J4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>0.0075</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>7989</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5">
+        <v>2296</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>99441</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>99441</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>99433</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4">
+        <v>96478</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>98875</v>
+      </c>
+      <c r="F5">
+        <v>566</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>160</v>
+      </c>
+      <c r="D6">
+        <v>0.001608994278014099</v>
+      </c>
+      <c r="E6">
+        <v>90733</v>
+      </c>
+      <c r="F6">
+        <v>8707</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>1783</v>
+      </c>
+      <c r="D7">
+        <v>0.01793022998561961</v>
+      </c>
+      <c r="E7">
+        <v>81018</v>
+      </c>
+      <c r="F7">
+        <v>18422</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>2965</v>
+      </c>
+      <c r="D8">
+        <v>0.02981667521444877</v>
+      </c>
+      <c r="E8">
+        <v>95664</v>
+      </c>
+      <c r="F8">
+        <v>3776</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>459</v>
+      </c>
+      <c r="F9">
+        <v>98982</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9">
+        <v>522</v>
+      </c>
+      <c r="I9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>98666</v>
+      </c>
+      <c r="F2">
+        <v>13984</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>112629</v>
+      </c>
+      <c r="K3">
+        <v>1.197833999112295</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>21</v>
+      </c>
+      <c r="N3">
+        <v>0.4971998996509814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>32951</v>
+      </c>
+      <c r="F4">
+        <v>79699</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4">
+        <v>527</v>
+      </c>
+      <c r="I4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>3095</v>
+      </c>
+      <c r="F5">
+        <v>109555</v>
+      </c>
+      <c r="G5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5">
+        <v>2033</v>
+      </c>
+      <c r="I5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>93318</v>
+      </c>
+      <c r="F6">
+        <v>19332</v>
+      </c>
+      <c r="G6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>5968</v>
+      </c>
+      <c r="F7">
+        <v>106682</v>
+      </c>
+      <c r="K7">
+        <v>120.6537390146471</v>
+      </c>
+      <c r="L7">
+        <v>0.85</v>
+      </c>
+      <c r="M7">
+        <v>6735</v>
+      </c>
+      <c r="N7">
+        <v>33721.41953116785</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>6999</v>
+      </c>
+      <c r="F8">
+        <v>105651</v>
+      </c>
+      <c r="K8">
+        <v>19.99031992898358</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>409.68</v>
+      </c>
+      <c r="N8">
+        <v>249.8424520578945</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>99440</v>
+      </c>
+      <c r="F2">
+        <v>4446</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>103857</v>
+      </c>
+      <c r="K3">
+        <v>1.092678512985388</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>29</v>
+      </c>
+      <c r="N3">
+        <v>0.4992606370214822</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>103881</v>
+      </c>
+      <c r="G4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4">
+        <v>76795</v>
+      </c>
+      <c r="I4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>103862</v>
+      </c>
+      <c r="K5">
+        <v>2.853348863176944</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>24</v>
+      </c>
+      <c r="N5">
+        <v>7.22024132387256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>29077</v>
+      </c>
+      <c r="F6">
+        <v>74809</v>
+      </c>
+      <c r="K6">
+        <v>154.1003804169956</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>13664.08</v>
+      </c>
+      <c r="N6">
+        <v>47303.66781639279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>98410</v>
+      </c>
+      <c r="F2">
+        <v>814</v>
+      </c>
+      <c r="G2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>98673</v>
+      </c>
+      <c r="F3">
+        <v>551</v>
+      </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>99219</v>
+      </c>
+      <c r="K4">
+        <v>4.08642062404257</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>1.815969514616923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>87656</v>
+      </c>
+      <c r="D5">
+        <v>0.8834153027493349</v>
+      </c>
+      <c r="E5">
+        <v>4527</v>
+      </c>
+      <c r="F5">
+        <v>94696</v>
+      </c>
+      <c r="G5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5">
+        <v>423</v>
+      </c>
+      <c r="I5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>58247</v>
+      </c>
+      <c r="D6">
+        <v>0.5870253164556962</v>
+      </c>
+      <c r="E6">
+        <v>36159</v>
+      </c>
+      <c r="F6">
+        <v>63064</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6">
+        <v>230</v>
+      </c>
+      <c r="I6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>636</v>
+      </c>
+      <c r="F7">
+        <v>98588</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7">
+        <v>463</v>
+      </c>
+      <c r="I7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>98248</v>
+      </c>
+      <c r="F8">
+        <v>976</v>
+      </c>
+      <c r="G8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>32951</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>610</v>
+      </c>
+      <c r="D3">
+        <v>0.018512336499651</v>
+      </c>
+      <c r="E3">
+        <v>73</v>
+      </c>
+      <c r="F3">
+        <v>32877</v>
+      </c>
+      <c r="G3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3">
+        <v>3029</v>
+      </c>
+      <c r="I3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>610</v>
+      </c>
+      <c r="D4">
+        <v>0.018512336499651</v>
+      </c>
+      <c r="E4">
+        <v>66</v>
+      </c>
+      <c r="F4">
+        <v>32884</v>
       </c>
       <c r="K4">
         <v>48.47694876472589</v>
@@ -1011,34 +3519,22 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>610</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.018512336499651</v>
       </c>
       <c r="E5">
-        <v>23</v>
+        <v>2960</v>
       </c>
       <c r="F5">
-        <v>3072</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5">
-        <v>1849</v>
-      </c>
-      <c r="I5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
+        <v>29990</v>
       </c>
       <c r="K5">
         <v>771.4952846232337</v>
@@ -1072,18 +3568,6 @@
       <c r="F6">
         <v>32931</v>
       </c>
-      <c r="G6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H6">
-        <v>230</v>
-      </c>
-      <c r="I6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
       <c r="K6">
         <v>2.18898611669398</v>
       </c>
@@ -1116,18 +3600,6 @@
       <c r="F7">
         <v>30746</v>
       </c>
-      <c r="G7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7">
-        <v>463</v>
-      </c>
-      <c r="I7" t="s">
-        <v>134</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
       <c r="K7">
         <v>2276.472487784151</v>
       </c>
@@ -1160,18 +3632,6 @@
       <c r="F8">
         <v>32851</v>
       </c>
-      <c r="G8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>135</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
       <c r="K8">
         <v>30.81507784758263</v>
       </c>
@@ -1204,18 +3664,6 @@
       <c r="F9">
         <v>32848</v>
       </c>
-      <c r="G9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9">
-        <v>522</v>
-      </c>
-      <c r="I9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
       <c r="K9">
         <v>16.93766123402835</v>
       </c>
@@ -1248,18 +3696,6 @@
       <c r="F10">
         <v>32855</v>
       </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>58</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
       <c r="K10">
         <v>23.1967282770342</v>
       </c>
@@ -1271,166 +3707,6 @@
       </c>
       <c r="N10">
         <v>145.9033873773299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11">
-        <v>778</v>
-      </c>
-      <c r="D11">
-        <v>0.9239904988123515</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>839</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>54</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>776</v>
-      </c>
-      <c r="D12">
-        <v>0.9216152019002375</v>
-      </c>
-      <c r="E12">
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <v>835</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>0.01187648456057007</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <v>838</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13">
-        <v>587</v>
-      </c>
-      <c r="I13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14">
-        <v>773</v>
-      </c>
-      <c r="D14">
-        <v>0.9180522565320665</v>
-      </c>
-      <c r="E14">
-        <v>33</v>
-      </c>
-      <c r="F14">
-        <v>808</v>
-      </c>
-      <c r="K14">
-        <v>233.0289855072464</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>2000</v>
-      </c>
-      <c r="N14">
-        <v>124172.0579710145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>27</v>
-      </c>
-      <c r="F15">
-        <v>815</v>
-      </c>
-      <c r="K15">
-        <v>73377.67933491686</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>50000000</v>
-      </c>
-      <c r="N15">
-        <v>3044324167681.025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>